<commit_message>
Added heater,tape and NTC
</commit_message>
<xml_diff>
--- a/mfg/BOM/bom-Vayu-prod-rev-p01.xlsx
+++ b/mfg/BOM/bom-Vayu-prod-rev-p01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\varun\Documents\EAGLE\projects\Vayu\mfg\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F07A126A-06E1-4FE2-9663-30A939CFD4F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA6E5074-A1C3-44EA-B612-FC5A74E09E52}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="345" yWindow="2775" windowWidth="38700" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="25695" yWindow="0" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="bom-Vayu-prod-rev-p01" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="100">
   <si>
     <t>Value</t>
   </si>
@@ -71,9 +71,6 @@
     <t>Molex</t>
   </si>
   <si>
-    <t>Sub-GHz antenna</t>
-  </si>
-  <si>
     <t>product-label</t>
   </si>
   <si>
@@ -119,9 +116,6 @@
     <t>LFB050CTP</t>
   </si>
   <si>
-    <t>Light Pipe Single Clear, Diffused Rigid Panel Mount, Press Fit, Front</t>
-  </si>
-  <si>
     <t>Mec, Front shell</t>
   </si>
   <si>
@@ -200,18 +194,6 @@
     <t>Vayu_AC_DC-PCBA</t>
   </si>
   <si>
-    <t>PCB, Vayu-R1A, Assembled</t>
-  </si>
-  <si>
-    <t>PCB, Vayu-i2c-R1A, Assembled</t>
-  </si>
-  <si>
-    <t>PCB, Vayu_AC_DC-R1A, Assembled</t>
-  </si>
-  <si>
-    <t>Aluminim tubes</t>
-  </si>
-  <si>
     <t>Tube, Aluminim, ID4mm, OD6mm, 166mm length</t>
   </si>
   <si>
@@ -285,6 +267,75 @@
   </si>
   <si>
     <t>magnet, Neodeam, 20mm x 10mm x 2mm</t>
+  </si>
+  <si>
+    <t>Aluminium tape</t>
+  </si>
+  <si>
+    <t>Aluminium tubes</t>
+  </si>
+  <si>
+    <t>tape, 50mm width, 250mm length, Metallic searing tape for high and low temperature channels, waterproof</t>
+  </si>
+  <si>
+    <t>Tesa</t>
+  </si>
+  <si>
+    <t>Tesa-60672</t>
+  </si>
+  <si>
+    <t>NTC-100K-probe</t>
+  </si>
+  <si>
+    <t>probe, NTC temperature probe, 100K, B3950 Thermistor, OD3mm Cartridge sensor</t>
+  </si>
+  <si>
+    <t>Used in 3d printer extruder hot ends</t>
+  </si>
+  <si>
+    <t>Polymide-film-heater</t>
+  </si>
+  <si>
+    <t>Heater, Polymide film, 12Volt, 10watts, 30mm x 90mm</t>
+  </si>
+  <si>
+    <t>LFB075CTP</t>
+  </si>
+  <si>
+    <t>Light Pipe, 3mm dia, 19mm length, Single Clear, Diffused Rigid Panel Mount, Press Fit, Front</t>
+  </si>
+  <si>
+    <t>Optinal Sub-GHz antenna</t>
+  </si>
+  <si>
+    <t>Vayu-i2c_R1A-PCBA</t>
+  </si>
+  <si>
+    <t>Vayu_AC_DC-R1A-PCBA</t>
+  </si>
+  <si>
+    <t>Vayu_wall_frame</t>
+  </si>
+  <si>
+    <t>Vayu_fan_shroude</t>
+  </si>
+  <si>
+    <t>Vayu_filter_cap_front</t>
+  </si>
+  <si>
+    <t>Vayu_heat_accumulator_shroude</t>
+  </si>
+  <si>
+    <t>Vayu_filter_cap_back</t>
+  </si>
+  <si>
+    <t>PCBA, Vayu-R1A, Assembled</t>
+  </si>
+  <si>
+    <t>PCBA, Vayu-i2c-R1A, Assembled</t>
+  </si>
+  <si>
+    <t>PCBA, Vayu_AC_DC-R1A, Assembled</t>
   </si>
 </sst>
 </file>
@@ -444,8 +495,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41D12416-A168-444F-B972-DB83B12B4CC0}" name="Table1" displayName="Table1" ref="A2:F26" totalsRowShown="0" headerRowDxfId="0">
-  <autoFilter ref="A2:F26" xr:uid="{41D12416-A168-444F-B972-DB83B12B4CC0}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{41D12416-A168-444F-B972-DB83B12B4CC0}" name="Table1" displayName="Table1" ref="A2:F29" totalsRowShown="0" headerRowDxfId="0">
+  <autoFilter ref="A2:F29" xr:uid="{41D12416-A168-444F-B972-DB83B12B4CC0}"/>
   <tableColumns count="6">
     <tableColumn id="1" xr3:uid="{8814CA96-3F33-4834-830E-2C96467059DE}" name="Value"/>
     <tableColumn id="2" xr3:uid="{FC617F48-2A96-4016-908A-4B8FC656328F}" name="Title"/>
@@ -724,22 +775,22 @@
   <dimension ref="A1:G34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="34" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="98.7109375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="49.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="10" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="B1" s="10"/>
       <c r="C1" s="10"/>
@@ -770,10 +821,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>26</v>
+        <v>87</v>
       </c>
       <c r="B3" t="s">
-        <v>27</v>
+        <v>88</v>
       </c>
       <c r="C3">
         <v>2</v>
@@ -782,7 +833,7 @@
         <v>6</v>
       </c>
       <c r="E3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -805,374 +856,449 @@
         <v>8</v>
       </c>
       <c r="F4" t="s">
-        <v>11</v>
+        <v>89</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
         <v>13</v>
       </c>
-      <c r="C5">
-        <v>1</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="E5" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
+      <c r="F5" t="s">
         <v>15</v>
-      </c>
-      <c r="F5" t="s">
-        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="E6" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="E7" t="s">
+        <v>92</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" t="s">
         <v>31</v>
       </c>
-      <c r="B8" t="s">
-        <v>33</v>
-      </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="E8" t="s">
+        <v>93</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>44</v>
+        <v>42</v>
+      </c>
+      <c r="E9" t="s">
+        <v>94</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>56</v>
       </c>
       <c r="C10">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E10" t="s">
-        <v>68</v>
-      </c>
-      <c r="F10" t="s">
-        <v>69</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="B11" t="s">
-        <v>46</v>
+        <v>54</v>
       </c>
       <c r="C11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D11" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E11" t="s">
-        <v>70</v>
-      </c>
-      <c r="F11" t="s">
-        <v>71</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B12" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="C12">
         <v>2</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>39</v>
+      </c>
+      <c r="E12" t="s">
+        <v>62</v>
+      </c>
+      <c r="F12" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="C13">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>72</v>
+        <v>39</v>
+      </c>
+      <c r="E13" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
         <v>40</v>
       </c>
       <c r="C14">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D14" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>38</v>
+        <v>16</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C15">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="D15" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>63</v>
+        <v>37</v>
       </c>
       <c r="B16" t="s">
-        <v>64</v>
+        <v>38</v>
       </c>
       <c r="C16">
         <v>4</v>
       </c>
       <c r="D16" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="B17" t="s">
-        <v>50</v>
+        <v>18</v>
       </c>
       <c r="C17">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="D17" t="s">
-        <v>49</v>
-      </c>
-      <c r="E17" t="s">
-        <v>48</v>
+        <v>66</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="B18" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C18">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>66</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>47</v>
+      </c>
+      <c r="E19" t="s">
+        <v>46</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="B20" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>67</v>
+      </c>
+      <c r="E20" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="B21" t="s">
-        <v>58</v>
+        <v>98</v>
       </c>
       <c r="C21">
-        <v>211</v>
+        <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="E21" t="s">
-        <v>66</v>
-      </c>
-      <c r="F21" t="s">
-        <v>67</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>60</v>
+        <v>99</v>
       </c>
       <c r="C22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>44</v>
+        <v>67</v>
+      </c>
+      <c r="E22" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
+        <v>78</v>
+      </c>
+      <c r="B23" t="s">
+        <v>52</v>
+      </c>
+      <c r="C23">
+        <v>211</v>
+      </c>
+      <c r="D23" t="s">
+        <v>59</v>
+      </c>
+      <c r="E23" t="s">
+        <v>60</v>
+      </c>
+      <c r="F23" t="s">
         <v>61</v>
-      </c>
-      <c r="B23" t="s">
-        <v>62</v>
-      </c>
-      <c r="C23">
-        <v>1</v>
-      </c>
-      <c r="D23" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B24" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E24" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="B25" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="C25">
         <v>1</v>
       </c>
       <c r="D25" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
+        <v>75</v>
+      </c>
+      <c r="B26" t="s">
+        <v>76</v>
+      </c>
+      <c r="C26">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>77</v>
+      </c>
+      <c r="B27" t="s">
+        <v>79</v>
+      </c>
+      <c r="C27">
+        <v>1</v>
+      </c>
+      <c r="D27" t="s">
+        <v>80</v>
+      </c>
+      <c r="E27" t="s">
         <v>81</v>
       </c>
-      <c r="B26" t="s">
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
         <v>82</v>
       </c>
-      <c r="C26">
-        <v>1</v>
-      </c>
-      <c r="D26" t="s">
-        <v>72</v>
+      <c r="B28" t="s">
+        <v>83</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28" t="s">
+        <v>66</v>
+      </c>
+      <c r="F28" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>85</v>
+      </c>
+      <c r="B29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29">
+        <v>1</v>
+      </c>
+      <c r="D29" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:6" ht="21" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B31" s="11"/>
       <c r="C31" s="11"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B32" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B32" s="4" t="s">
+      <c r="C32" s="5" t="s">
         <v>22</v>
-      </c>
-      <c r="C32" s="5" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B33" s="7">
         <v>45638</v>
       </c>
       <c r="C33" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>